<commit_message>
Updating to include new variables added to files
</commit_message>
<xml_diff>
--- a/data/static_tables/metric_structure_newcolumns.xlsx
+++ b/data/static_tables/metric_structure_newcolumns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\russelle\egrid\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF01A056-45B3-4CE5-A9A9-8BE0FB888A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B064B5-0D02-41D8-872E-57A8FB6B7635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UNT21" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6194" uniqueCount="2924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6212" uniqueCount="2932">
   <si>
     <t>Name</t>
   </si>
@@ -8798,9 +8798,6 @@
     <t>PLC2ERA</t>
   </si>
   <si>
-    <t>Stack or Flue ID</t>
-  </si>
-  <si>
     <t>Stack Flue Status</t>
   </si>
   <si>
@@ -8829,6 +8826,33 @@
   </si>
   <si>
     <t>CHPCO2E</t>
+  </si>
+  <si>
+    <t>STACKHT</t>
+  </si>
+  <si>
+    <t>PLGENATO</t>
+  </si>
+  <si>
+    <t>PLGENATO2</t>
+  </si>
+  <si>
+    <t>Plant annual other nonrenewables net generation (MWh)</t>
+  </si>
+  <si>
+    <t>Plant annual other nonrenewables net generation (GJ)</t>
+  </si>
+  <si>
+    <t>Plant annual other noncombustion net generation (MWh)</t>
+  </si>
+  <si>
+    <t>PLGENACO</t>
+  </si>
+  <si>
+    <t>Plant annual other noncombustion net generation (GJ)</t>
+  </si>
+  <si>
+    <t>PLGENACO2</t>
   </si>
 </sst>
 </file>
@@ -9748,11 +9772,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -9990,7 +10014,7 @@
       </c>
       <c r="E18" s="139"/>
     </row>
-    <row r="19" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
         <v>42</v>
       </c>
@@ -10181,26 +10205,19 @@
       <c r="E34" s="139"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="152" t="s">
         <v>2914</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
+      <c r="B35" s="153" t="s">
+        <v>2923</v>
+      </c>
+      <c r="C35" s="154" t="s">
+        <v>2916</v>
+      </c>
+      <c r="D35" s="154" t="s">
+        <v>2915</v>
+      </c>
       <c r="E35" s="139"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="152" t="s">
-        <v>2915</v>
-      </c>
-      <c r="B36" s="153"/>
-      <c r="C36" s="154" t="s">
-        <v>2917</v>
-      </c>
-      <c r="D36" s="154" t="s">
-        <v>2916</v>
-      </c>
-      <c r="E36" s="139"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10489,11 +10506,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IN179"/>
+  <dimension ref="A1:IN183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E118" sqref="E118"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12567,10 +12584,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="38" t="s">
+        <v>2917</v>
+      </c>
+      <c r="B100" s="70" t="s">
         <v>2918</v>
-      </c>
-      <c r="B100" s="70" t="s">
-        <v>2919</v>
       </c>
       <c r="C100" s="130" t="s">
         <v>40</v>
@@ -12846,10 +12863,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="72" t="s">
+        <v>2919</v>
+      </c>
+      <c r="B121" s="73" t="s">
         <v>2920</v>
-      </c>
-      <c r="B121" s="73" t="s">
-        <v>2921</v>
       </c>
       <c r="C121" s="131" t="s">
         <v>40</v>
@@ -12981,10 +12998,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="155" t="s">
+        <v>2921</v>
+      </c>
+      <c r="B130" s="73" t="s">
         <v>2922</v>
-      </c>
-      <c r="B130" s="73" t="s">
-        <v>2923</v>
       </c>
       <c r="C130" s="131" t="s">
         <v>40</v>
@@ -13395,10 +13412,10 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="77" t="s">
-        <v>397</v>
+        <v>2926</v>
       </c>
       <c r="B156" s="78" t="s">
-        <v>398</v>
+        <v>2924</v>
       </c>
       <c r="C156" s="78" t="s">
         <v>93</v>
@@ -13410,10 +13427,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="77" t="s">
-        <v>399</v>
+        <v>2927</v>
       </c>
       <c r="B157" s="78" t="s">
-        <v>400</v>
+        <v>2925</v>
       </c>
       <c r="C157" s="78" t="s">
         <v>34</v>
@@ -13426,63 +13443,63 @@
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" s="79" t="s">
+      <c r="A158" s="77" t="s">
+        <v>397</v>
+      </c>
+      <c r="B158" s="78" t="s">
+        <v>398</v>
+      </c>
+      <c r="C158" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="D158" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="E158" s="144"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="77" t="s">
+        <v>399</v>
+      </c>
+      <c r="B159" s="78" t="s">
+        <v>400</v>
+      </c>
+      <c r="C159" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="D159" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="E159" s="144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="79" t="s">
         <v>401</v>
       </c>
-      <c r="B158" s="80" t="s">
+      <c r="B160" s="80" t="s">
         <v>402</v>
       </c>
-      <c r="C158" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="D158" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="E158" s="144"/>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" s="79" t="s">
+      <c r="C160" s="80" t="s">
+        <v>93</v>
+      </c>
+      <c r="D160" s="80" t="s">
+        <v>93</v>
+      </c>
+      <c r="E160" s="144"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="79" t="s">
         <v>403</v>
       </c>
-      <c r="B159" s="80" t="s">
+      <c r="B161" s="80" t="s">
         <v>404</v>
       </c>
-      <c r="C159" s="80" t="s">
+      <c r="C161" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="D159" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="E159" s="144" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="81" t="s">
-        <v>405</v>
-      </c>
-      <c r="B160" s="82" t="s">
-        <v>406</v>
-      </c>
-      <c r="C160" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="D160" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="E160" s="144"/>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" s="81" t="s">
-        <v>407</v>
-      </c>
-      <c r="B161" s="82" t="s">
-        <v>408</v>
-      </c>
-      <c r="C161" s="148" t="s">
-        <v>34</v>
-      </c>
-      <c r="D161" s="148" t="s">
+      <c r="D161" s="80" t="s">
         <v>93</v>
       </c>
       <c r="E161" s="144" t="s">
@@ -13491,10 +13508,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="81" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B162" s="82" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C162" s="148" t="s">
         <v>93</v>
@@ -13506,10 +13523,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="81" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B163" s="82" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C163" s="148" t="s">
         <v>34</v>
@@ -13522,71 +13539,75 @@
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="83" t="s">
-        <v>413</v>
-      </c>
-      <c r="B164" s="84" t="s">
-        <v>414</v>
-      </c>
-      <c r="C164" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="D164" s="132" t="s">
-        <v>415</v>
+      <c r="A164" s="81" t="s">
+        <v>409</v>
+      </c>
+      <c r="B164" s="82" t="s">
+        <v>410</v>
+      </c>
+      <c r="C164" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="D164" s="148" t="s">
+        <v>93</v>
       </c>
       <c r="E164" s="144"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="83" t="s">
-        <v>416</v>
-      </c>
-      <c r="B165" s="84" t="s">
-        <v>417</v>
-      </c>
-      <c r="C165" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="D165" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="E165" s="144"/>
+      <c r="A165" s="81" t="s">
+        <v>411</v>
+      </c>
+      <c r="B165" s="82" t="s">
+        <v>412</v>
+      </c>
+      <c r="C165" s="148" t="s">
+        <v>34</v>
+      </c>
+      <c r="D165" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="E165" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" s="83" t="s">
-        <v>418</v>
-      </c>
-      <c r="B166" s="84" t="s">
-        <v>419</v>
-      </c>
-      <c r="C166" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="D166" s="132" t="s">
-        <v>415</v>
+      <c r="A166" s="81" t="s">
+        <v>2928</v>
+      </c>
+      <c r="B166" s="82" t="s">
+        <v>2929</v>
+      </c>
+      <c r="C166" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="D166" s="148" t="s">
+        <v>93</v>
       </c>
       <c r="E166" s="144"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" s="83" t="s">
-        <v>420</v>
-      </c>
-      <c r="B167" s="84" t="s">
-        <v>421</v>
-      </c>
-      <c r="C167" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="D167" s="132" t="s">
-        <v>415</v>
-      </c>
-      <c r="E167" s="144"/>
+      <c r="A167" s="81" t="s">
+        <v>2930</v>
+      </c>
+      <c r="B167" s="82" t="s">
+        <v>2931</v>
+      </c>
+      <c r="C167" s="148" t="s">
+        <v>34</v>
+      </c>
+      <c r="D167" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="E167" s="144" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="83" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="B168" s="84" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="C168" s="132" t="s">
         <v>415</v>
@@ -13598,10 +13619,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="83" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B169" s="84" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="C169" s="132" t="s">
         <v>415</v>
@@ -13613,10 +13634,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="83" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B170" s="84" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="C170" s="132" t="s">
         <v>415</v>
@@ -13628,10 +13649,10 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="83" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B171" s="84" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="C171" s="132" t="s">
         <v>415</v>
@@ -13643,10 +13664,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="83" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B172" s="84" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C172" s="132" t="s">
         <v>415</v>
@@ -13658,10 +13679,10 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="83" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="B173" s="84" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="C173" s="132" t="s">
         <v>415</v>
@@ -13673,10 +13694,10 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="83" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B174" s="84" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C174" s="132" t="s">
         <v>415</v>
@@ -13687,79 +13708,139 @@
       <c r="E174" s="144"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A175" s="85" t="s">
+      <c r="A175" s="83" t="s">
+        <v>428</v>
+      </c>
+      <c r="B175" s="84" t="s">
+        <v>429</v>
+      </c>
+      <c r="C175" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="D175" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E175" s="144"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" s="83" t="s">
+        <v>430</v>
+      </c>
+      <c r="B176" s="84" t="s">
+        <v>431</v>
+      </c>
+      <c r="C176" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="D176" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E176" s="144"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" s="83" t="s">
+        <v>432</v>
+      </c>
+      <c r="B177" s="84" t="s">
+        <v>433</v>
+      </c>
+      <c r="C177" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="D177" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E177" s="144"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" s="83" t="s">
+        <v>434</v>
+      </c>
+      <c r="B178" s="84" t="s">
+        <v>435</v>
+      </c>
+      <c r="C178" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="D178" s="132" t="s">
+        <v>415</v>
+      </c>
+      <c r="E178" s="144"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" s="85" t="s">
         <v>436</v>
       </c>
-      <c r="B175" s="86" t="s">
+      <c r="B179" s="86" t="s">
         <v>437</v>
       </c>
-      <c r="C175" s="133" t="s">
+      <c r="C179" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="D175" s="133" t="s">
+      <c r="D179" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="E175" s="144"/>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A176" s="85" t="s">
+      <c r="E179" s="144"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" s="85" t="s">
         <v>438</v>
       </c>
-      <c r="B176" s="86" t="s">
+      <c r="B180" s="86" t="s">
         <v>439</v>
       </c>
-      <c r="C176" s="133" t="s">
+      <c r="C180" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="D176" s="133" t="s">
+      <c r="D180" s="133" t="s">
         <v>415</v>
       </c>
-      <c r="E176" s="144"/>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177" s="87" t="s">
+      <c r="E180" s="144"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" s="87" t="s">
         <v>440</v>
       </c>
-      <c r="B177" s="88" t="s">
+      <c r="B181" s="88" t="s">
         <v>441</v>
       </c>
-      <c r="C177" s="134" t="s">
+      <c r="C181" s="134" t="s">
         <v>415</v>
       </c>
-      <c r="D177" s="134" t="s">
+      <c r="D181" s="134" t="s">
         <v>415</v>
       </c>
-      <c r="E177" s="144"/>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A178" s="89" t="s">
+      <c r="E181" s="144"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="89" t="s">
         <v>442</v>
       </c>
-      <c r="B178" s="90" t="s">
+      <c r="B182" s="90" t="s">
         <v>443</v>
       </c>
-      <c r="C178" s="135" t="s">
+      <c r="C182" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="D178" s="135" t="s">
+      <c r="D182" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="E178" s="144"/>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A179" s="89" t="s">
+      <c r="E182" s="144"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="89" t="s">
         <v>444</v>
       </c>
-      <c r="B179" s="90" t="s">
+      <c r="B183" s="90" t="s">
         <v>445</v>
       </c>
-      <c r="C179" s="135" t="s">
+      <c r="C183" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="D179" s="135" t="s">
+      <c r="D183" s="135" t="s">
         <v>415</v>
       </c>
-      <c r="E179" s="144"/>
+      <c r="E183" s="144"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13771,9 +13852,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:IN248"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" activeCellId="2" sqref="A42:XFD42 A43:XFD43 A44:XFD44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -33476,6 +33557,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6c854b04-c9c6-4391-adbe-2e73191270e7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="059b9c67-646b-4b4e-9ab1-2b1c805d0390">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AD6200282E8E804DB7E47654D11346C2" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="334b3f607926cb22599f187b4c015ce1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="059b9c67-646b-4b4e-9ab1-2b1c805d0390" xmlns:ns3="c05e7bd6-26a7-41a1-805c-893279a3732f" xmlns:ns4="6c854b04-c9c6-4391-adbe-2e73191270e7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fe548b9ff7492f3109b4e0b4a8efc8f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
@@ -33735,27 +33836,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6c854b04-c9c6-4391-adbe-2e73191270e7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="059b9c67-646b-4b4e-9ab1-2b1c805d0390">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA6965B-A23A-4F60-9CAE-00FD555BD4D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2EA77E-CA9B-4563-9A5E-2F50B3C8BA13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c854b04-c9c6-4391-adbe-2e73191270e7"/>
+    <ds:schemaRef ds:uri="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FE51207-01AF-400E-9D05-58F426138751}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33773,23 +33873,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2EA77E-CA9B-4563-9A5E-2F50B3C8BA13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c854b04-c9c6-4391-adbe-2e73191270e7"/>
-    <ds:schemaRef ds:uri="059b9c67-646b-4b4e-9ab1-2b1c805d0390"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCA6965B-A23A-4F60-9CAE-00FD555BD4D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>